<commit_message>
Adicionando formatação condicional na aba Vendas
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" state="visible" r:id="rId1"/>
@@ -69,7 +69,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -80,6 +80,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -102,7 +107,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -118,6 +123,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -330,11 +338,11 @@
         </ser>
         <gapWidth val="150"/>
         <overlap val="0"/>
-        <axId val="21987210"/>
-        <axId val="14347220"/>
+        <axId val="69255061"/>
+        <axId val="97019451"/>
       </barChart>
       <catAx>
-        <axId val="21987210"/>
+        <axId val="69255061"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -404,7 +412,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="14347220"/>
+        <crossAx val="97019451"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -412,7 +420,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="14347220"/>
+        <axId val="97019451"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -492,7 +500,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="21987210"/>
+        <crossAx val="69255061"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -544,484 +552,19 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1300" b="0" strike="noStrike">
-                <a:uFillTx/>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Quantidade de vendas por produto</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-      <spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <varyColors val="0"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>Vendas!B1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Quantidade</v>
-                </pt>
-              </strCache>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike">
-                    <a:uFillTx/>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </txPr>
-            <showLegendKey val="0"/>
-            <showVal val="0"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showLeaderLines val="1"/>
-          </dLbls>
-          <cat>
-            <strRef>
-              <f>Vendas!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Morango</v>
-                </pt>
-                <pt idx="1">
-                  <v>Maçã</v>
-                </pt>
-                <pt idx="2">
-                  <v>Manga</v>
-                </pt>
-                <pt idx="3">
-                  <v>Kiwi</v>
-                </pt>
-                <pt idx="4">
-                  <v>Uva</v>
-                </pt>
-              </strCache>
-            </strRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>Vendas!$B$2:$B$6</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>15</v>
-                </pt>
-                <pt idx="1">
-                  <v>2</v>
-                </pt>
-                <pt idx="2">
-                  <v>6</v>
-                </pt>
-                <pt idx="3">
-                  <v>5</v>
-                </pt>
-                <pt idx="4">
-                  <v>11</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <overlap val="0"/>
-        <axId val="36586133"/>
-        <axId val="45431821"/>
-      </barChart>
-      <catAx>
-        <axId val="36586133"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1300" b="0" strike="noStrike">
-                    <a:uFillTx/>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Produto</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-          <overlay val="0"/>
-          <spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-        </title>
-        <numFmt formatCode="General" sourceLinked="1"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-          </a:p>
-        </txPr>
-        <crossAx val="45431821"/>
-        <crosses val="autoZero"/>
-        <auto val="1"/>
-        <lblAlgn val="ctr"/>
-        <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
-      </catAx>
-      <valAx>
-        <axId val="45431821"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines>
-          <spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-        </majorGridlines>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1300" b="0" strike="noStrike">
-                    <a:uFillTx/>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Vendas por produto</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-          <overlay val="0"/>
-          <spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-        </title>
-        <numFmt formatCode="General" sourceLinked="1"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-          </a:p>
-        </txPr>
-        <crossAx val="36586133"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-      <overlay val="0"/>
-      <spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-      <txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1000" b="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
-        </a:p>
-      </txPr>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-  <spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Quantidade de vendas por produto</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Vendas'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Vendas'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Vendas'!$B$2:$B$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Produto</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Vendas por produto</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
-      <col>4</col>
+      <col>0</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
     <to>
-      <col>12</col>
-      <colOff>507600</colOff>
-      <row>28</row>
+      <col>3</col>
+      <colOff>536040</colOff>
+      <row>21</row>
       <rowOff>32400</rowOff>
     </to>
     <graphicFrame>
@@ -1038,60 +581,6 @@
     </graphicFrame>
     <clientData/>
   </twoCellAnchor>
-  <twoCellAnchor editAs="oneCell">
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <to>
-      <col>12</col>
-      <colOff>507600</colOff>
-      <row>28</row>
-      <rowOff>32400</rowOff>
-    </to>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="2" name="Chart 2"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </twoCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>7</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1278,7 +767,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1340,7 +829,7 @@
       <c r="C3" s="3" t="n">
         <v>7.92</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="6" t="n">
         <v>15.84</v>
       </c>
     </row>
@@ -1356,7 +845,7 @@
       <c r="C4" s="3" t="n">
         <v>3.52</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>21.12</v>
       </c>
     </row>
@@ -1372,7 +861,7 @@
       <c r="C5" s="3" t="n">
         <v>8.539999999999999</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>42.7</v>
       </c>
     </row>
@@ -1388,7 +877,7 @@
       <c r="C6" s="3" t="n">
         <v>5.7</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="6" t="n">
         <v>62.7</v>
       </c>
     </row>
@@ -1396,7 +885,6 @@
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1408,8 +896,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
Renomeando os arquivos e adicionando novas abas na planilha 'dados'
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -4,11 +4,15 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Relatorio" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Janeiro" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Fevereiro" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Março" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Resumo" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -69,7 +73,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -80,11 +84,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -107,7 +106,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -117,6 +116,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -124,7 +126,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -267,11 +269,14 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
@@ -281,6 +286,7 @@
                 </a:r>
               </a:p>
             </txPr>
+            <dLblPos val="outEnd"/>
             <showLegendKey val="0"/>
             <showVal val="0"/>
             <showCatName val="0"/>
@@ -338,11 +344,11 @@
         </ser>
         <gapWidth val="150"/>
         <overlap val="0"/>
-        <axId val="69255061"/>
-        <axId val="97019451"/>
+        <axId val="78458506"/>
+        <axId val="76833855"/>
       </barChart>
       <catAx>
-        <axId val="69255061"/>
+        <axId val="78458506"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -382,7 +388,7 @@
             </a:ln>
           </spPr>
         </title>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <numFmt formatCode="General" sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
@@ -412,7 +418,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="97019451"/>
+        <crossAx val="76833855"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -420,7 +426,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="97019451"/>
+        <axId val="76833855"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -470,7 +476,7 @@
             </a:ln>
           </spPr>
         </title>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <numFmt formatCode="General" sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
@@ -500,7 +506,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="69255061"/>
+        <crossAx val="78458506"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -563,9 +569,9 @@
     </from>
     <to>
       <col>3</col>
-      <colOff>536040</colOff>
+      <colOff>533520</colOff>
       <row>21</row>
-      <rowOff>32400</rowOff>
+      <rowOff>29880</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -767,117 +773,117 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="9" customWidth="1" style="3" min="1" max="1"/>
-    <col width="12" customWidth="1" style="3" min="2" max="2"/>
-    <col width="16" customWidth="1" style="3" min="3" max="3"/>
-    <col width="7" customWidth="1" style="3" min="4" max="4"/>
+    <col width="9" customWidth="1" style="4" min="1" max="1"/>
+    <col width="12" customWidth="1" style="4" min="2" max="2"/>
+    <col width="16" customWidth="1" style="4" min="3" max="3"/>
+    <col width="7" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>10.36</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>155.4</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="4">
-      <c r="A3" s="3" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>7.92</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="7" t="n">
         <v>15.84</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="4">
-      <c r="A4" s="3" t="inlineStr">
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>3.52</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="7" t="n">
         <v>21.12</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="4">
-      <c r="A5" s="3" t="inlineStr">
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>8.539999999999999</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>42.7</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="4">
-      <c r="A6" s="3" t="inlineStr">
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>5.7</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>62.7</v>
       </c>
     </row>
@@ -894,47 +900,102 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="23" customWidth="1" style="3" min="1" max="3"/>
+    <col width="23" customWidth="1" style="4" min="1" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Total de vendas</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Produto mais vendido</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Produto mais rentável</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="3" t="n">
-        <v>297.76</v>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Morango</t>
-        </is>
+      <c r="B3" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Uva</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>8.380000000000001</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>7.46</v>
       </c>
     </row>
   </sheetData>
@@ -943,4 +1004,363 @@
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Uva</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Morango</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>19</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Morango</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Uva</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6.88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Morango</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8.630000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Uva</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculando dinamicamente os dados da coluna 'Total' de cada aba da planilha
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -282,7 +282,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -414,7 +414,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -502,7 +502,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -535,7 +535,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
         </a:p>
       </txPr>
@@ -819,8 +819,9 @@
       <c r="C2" s="4" t="n">
         <v>10.36</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>155.4</v>
+      <c r="D2" s="4">
+        <f>B2*C2</f>
+        <v/>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="5">
@@ -835,8 +836,9 @@
       <c r="C3" s="4" t="n">
         <v>7.92</v>
       </c>
-      <c r="D3" s="7" t="n">
-        <v>15.84</v>
+      <c r="D3" s="7">
+        <f>B3*C3</f>
+        <v/>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="5">
@@ -851,8 +853,9 @@
       <c r="C4" s="4" t="n">
         <v>3.52</v>
       </c>
-      <c r="D4" s="7" t="n">
-        <v>21.12</v>
+      <c r="D4" s="7">
+        <f>B4*C4</f>
+        <v/>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="5">
@@ -867,8 +870,9 @@
       <c r="C5" s="4" t="n">
         <v>8.539999999999999</v>
       </c>
-      <c r="D5" s="7" t="n">
-        <v>42.7</v>
+      <c r="D5" s="7">
+        <f>B5*C5</f>
+        <v/>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="5">
@@ -883,8 +887,9 @@
       <c r="C6" s="4" t="n">
         <v>5.7</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>62.7</v>
+      <c r="D6" s="7">
+        <f>B6*C6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -945,6 +950,10 @@
       <c r="C2" s="4" t="n">
         <v>7.3</v>
       </c>
+      <c r="D2" s="4">
+        <f>B2*C2</f>
+        <v/>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="5">
       <c r="A3" s="4" t="inlineStr">
@@ -958,6 +967,10 @@
       <c r="C3" s="4" t="n">
         <v>7.14</v>
       </c>
+      <c r="D3" s="4">
+        <f>B3*C3</f>
+        <v/>
+      </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="5">
       <c r="A4" s="4" t="inlineStr">
@@ -971,6 +984,10 @@
       <c r="C4" s="4" t="n">
         <v>8.380000000000001</v>
       </c>
+      <c r="D4" s="4">
+        <f>B4*C4</f>
+        <v/>
+      </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="5">
       <c r="A5" s="4" t="inlineStr">
@@ -984,6 +1001,10 @@
       <c r="C5" s="4" t="n">
         <v>2.61</v>
       </c>
+      <c r="D5" s="4">
+        <f>B5*C5</f>
+        <v/>
+      </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="5">
       <c r="A6" s="4" t="inlineStr">
@@ -996,6 +1017,10 @@
       </c>
       <c r="C6" s="4" t="n">
         <v>7.46</v>
+      </c>
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1021,90 +1046,110 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4" t="n">
         <v>5.14</v>
       </c>
+      <c r="D2" s="4">
+        <f>B2*C2</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="4" t="n">
         <v>1.43</v>
       </c>
+      <c r="D3" s="4">
+        <f>B3*C3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4" t="n">
         <v>5.19</v>
       </c>
+      <c r="D4" s="4">
+        <f>B4*C4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="4" t="n">
         <v>6.95</v>
       </c>
+      <c r="D5" s="4">
+        <f>B5*C5</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="4" t="n">
         <v>3.34</v>
+      </c>
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1127,90 +1172,110 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4" t="n">
         <v>1.73</v>
       </c>
+      <c r="D2" s="4">
+        <f>B2*C2</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="4" t="n">
         <v>9.68</v>
       </c>
+      <c r="D3" s="4">
+        <f>B3*C3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4" t="n">
         <v>9.83</v>
       </c>
+      <c r="D4" s="4">
+        <f>B4*C4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="4" t="n">
         <v>4.37</v>
       </c>
+      <c r="D5" s="4">
+        <f>B5*C5</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="4" t="n">
         <v>6.88</v>
+      </c>
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1233,90 +1298,110 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4" t="n">
         <v>5.41</v>
       </c>
+      <c r="D2" s="4">
+        <f>B2*C2</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="4" t="n">
         <v>8.630000000000001</v>
       </c>
+      <c r="D3" s="4">
+        <f>B3*C3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4" t="n">
         <v>1.25</v>
       </c>
+      <c r="D4" s="4">
+        <f>B4*C4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="4" t="n">
         <v>7.05</v>
       </c>
+      <c r="D5" s="4">
+        <f>B5*C5</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="4" t="n">
         <v>5.49</v>
+      </c>
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1339,22 +1424,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>

</xml_diff>

<commit_message>
Adicionando formatação nas abas Janeiro, Fevereiro e Março. E adicionando os nomes de produtos de forma ordenada alfabeticamente, na aba Resumo
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -72,8 +72,12 @@
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -84,6 +88,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -106,7 +115,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -128,6 +137,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1044,24 +1056,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" style="5" min="1" max="1"/>
+    <col width="14" customWidth="1" style="5" min="2" max="2"/>
+    <col width="18" customWidth="1" style="5" min="3" max="3"/>
+    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1170,24 +1188,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" style="5" min="1" max="1"/>
+    <col width="14" customWidth="1" style="5" min="2" max="2"/>
+    <col width="18" customWidth="1" style="5" min="3" max="3"/>
+    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1296,24 +1320,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" style="5" min="1" max="1"/>
+    <col width="14" customWidth="1" style="5" min="2" max="2"/>
+    <col width="18" customWidth="1" style="5" min="3" max="3"/>
+    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1415,33 +1445,74 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" style="5" min="1" max="1"/>
+    <col width="14" customWidth="1" style="5" min="2" max="2"/>
+    <col width="18" customWidth="1" style="5" min="3" max="3"/>
+    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Morango</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Uva</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionando as quantidades somadas dos meses de Janeiro, Fevereiro e Março, na planilha resumo
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -72,12 +72,8 @@
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -88,11 +84,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -115,7 +106,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -137,9 +128,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -294,7 +282,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t>None</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </txPr>
@@ -356,11 +344,11 @@
         </ser>
         <gapWidth val="150"/>
         <overlap val="0"/>
-        <axId val="78458506"/>
-        <axId val="76833855"/>
+        <axId val="65960605"/>
+        <axId val="14387934"/>
       </barChart>
       <catAx>
-        <axId val="78458506"/>
+        <axId val="65960605"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -426,11 +414,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="76833855"/>
+        <crossAx val="14387934"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -438,7 +426,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="76833855"/>
+        <axId val="14387934"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -514,11 +502,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="78458506"/>
+        <crossAx val="65960605"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -547,7 +535,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t>None</a:t>
+            <a:t/>
           </a:r>
         </a:p>
       </txPr>
@@ -581,9 +569,9 @@
     </from>
     <to>
       <col>3</col>
-      <colOff>533520</colOff>
+      <colOff>532800</colOff>
       <row>21</row>
-      <rowOff>29880</rowOff>
+      <rowOff>29160</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -919,7 +907,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1045,47 +1033,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11" customWidth="1" style="5" min="1" max="1"/>
-    <col width="14" customWidth="1" style="5" min="2" max="2"/>
-    <col width="18" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+    <col width="11" customWidth="1" style="4" min="1" max="1"/>
+    <col width="14" customWidth="1" style="4" min="2" max="2"/>
+    <col width="18" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1" s="5">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
@@ -1102,7 +1090,7 @@
         <v/>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1" s="5">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
@@ -1119,7 +1107,7 @@
         <v/>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="5">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
@@ -1136,7 +1124,7 @@
         <v/>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
@@ -1153,7 +1141,7 @@
         <v/>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1" s="5">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
@@ -1171,53 +1159,55 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11" customWidth="1" style="5" min="1" max="1"/>
-    <col width="14" customWidth="1" style="5" min="2" max="2"/>
-    <col width="18" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+    <col width="11" customWidth="1" style="4" min="1" max="1"/>
+    <col width="14" customWidth="1" style="4" min="2" max="2"/>
+    <col width="18" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1" s="5">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
@@ -1234,7 +1224,7 @@
         <v/>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1" s="5">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
@@ -1251,7 +1241,7 @@
         <v/>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="5">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
@@ -1268,7 +1258,7 @@
         <v/>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
@@ -1285,7 +1275,7 @@
         <v/>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1" s="5">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
@@ -1303,53 +1293,55 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11" customWidth="1" style="5" min="1" max="1"/>
-    <col width="14" customWidth="1" style="5" min="2" max="2"/>
-    <col width="18" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+    <col width="11" customWidth="1" style="4" min="1" max="1"/>
+    <col width="14" customWidth="1" style="4" min="2" max="2"/>
+    <col width="18" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1" s="5">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
@@ -1366,7 +1358,7 @@
         <v/>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1" s="5">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
@@ -1383,7 +1375,7 @@
         <v/>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="5">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
@@ -1400,7 +1392,7 @@
         <v/>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
@@ -1417,7 +1409,7 @@
         <v/>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1" s="5">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
@@ -1435,88 +1427,107 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11" customWidth="1" style="5" min="1" max="1"/>
-    <col width="14" customWidth="1" style="5" min="2" max="2"/>
-    <col width="18" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9" customWidth="1" style="5" min="4" max="4"/>
+    <col width="11" customWidth="1" style="4" min="1" max="1"/>
+    <col width="14" customWidth="1" style="4" min="2" max="2"/>
+    <col width="18" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Produto</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Preço Unitário</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Kiwi</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="B2" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="B3" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Maçã</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="B4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Morango</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="B5" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionando o preço unitário médio por produto na aba 'Resumo'
</commit_message>
<xml_diff>
--- a/frutas/dados.xlsx
+++ b/frutas/dados.xlsx
@@ -282,7 +282,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -344,11 +344,11 @@
         </ser>
         <gapWidth val="150"/>
         <overlap val="0"/>
-        <axId val="65960605"/>
-        <axId val="14387934"/>
+        <axId val="75384383"/>
+        <axId val="95004741"/>
       </barChart>
       <catAx>
-        <axId val="65960605"/>
+        <axId val="75384383"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -414,11 +414,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="14387934"/>
+        <crossAx val="95004741"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -426,7 +426,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="14387934"/>
+        <axId val="95004741"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -502,11 +502,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="65960605"/>
+        <crossAx val="75384383"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -535,7 +535,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
         </a:p>
       </txPr>
@@ -569,9 +569,9 @@
     </from>
     <to>
       <col>3</col>
-      <colOff>532800</colOff>
+      <colOff>532440</colOff>
       <row>21</row>
-      <rowOff>29160</rowOff>
+      <rowOff>28800</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1442,7 +1442,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
@@ -1481,8 +1481,11 @@
           <t>Kiwi</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>37</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4.600000000000001</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="5">
@@ -1491,8 +1494,11 @@
           <t>Manga</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>51</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>6.760000000000001</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="5">
@@ -1501,8 +1507,11 @@
           <t>Maçã</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>28</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>4.04</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="5">
@@ -1511,8 +1520,11 @@
           <t>Morango</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>46</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>8.470000000000001</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="5">
@@ -1521,8 +1533,11 @@
           <t>Uva</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>25</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>3.586666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>